<commit_message>
Insert excel of hybrid groups into DB
</commit_message>
<xml_diff>
--- a/backend/scripts/excel_example.xlsx
+++ b/backend/scripts/excel_example.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25915"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ACDE7DA5-15DE-45CA-90AD-455BD508DBF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FF87FAF7-3C52-47E8-84E3-5A6167103F93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="13">
   <si>
     <t>Group name 1</t>
   </si>
@@ -39,25 +39,34 @@
     <t>OFF</t>
   </si>
   <si>
-    <t>name 1</t>
+    <t>黃國彰</t>
   </si>
   <si>
     <t>id 1</t>
   </si>
   <si>
-    <t>name 2</t>
+    <t>黃健原</t>
   </si>
   <si>
     <t>id 2</t>
   </si>
   <si>
-    <t>name 3</t>
+    <t>陳音儕</t>
   </si>
   <si>
     <t>id 3</t>
   </si>
   <si>
     <t>Group name 2</t>
+  </si>
+  <si>
+    <t>陳雅玲</t>
+  </si>
+  <si>
+    <t>陳維祥</t>
+  </si>
+  <si>
+    <t>陳素珍</t>
   </si>
 </sst>
 </file>
@@ -423,7 +432,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -741,7 +750,7 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B15" t="s">
         <v>4</v>
@@ -770,7 +779,7 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
@@ -793,7 +802,7 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B17" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Update group from excel, see changes live
</commit_message>
<xml_diff>
--- a/backend/scripts/excel_example.xlsx
+++ b/backend/scripts/excel_example.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25915"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25917"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FF87FAF7-3C52-47E8-84E3-5A6167103F93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FABDA125-8025-4C6B-9553-632CF6D37E62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,9 +28,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="13">
-  <si>
-    <t>Group name 1</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
+  <si>
+    <t>awkward workers</t>
   </si>
   <si>
     <t>ON</t>
@@ -39,41 +39,29 @@
     <t>OFF</t>
   </si>
   <si>
-    <t>黃國彰</t>
-  </si>
-  <si>
-    <t>id 1</t>
-  </si>
-  <si>
-    <t>黃健原</t>
-  </si>
-  <si>
-    <t>id 2</t>
-  </si>
-  <si>
-    <t>陳音儕</t>
-  </si>
-  <si>
-    <t>id 3</t>
-  </si>
-  <si>
-    <t>Group name 2</t>
-  </si>
-  <si>
-    <t>陳雅玲</t>
-  </si>
-  <si>
-    <t>陳維祥</t>
-  </si>
-  <si>
-    <t>陳素珍</t>
+    <t>李沄蒨</t>
+  </si>
+  <si>
+    <t>D049</t>
+  </si>
+  <si>
+    <t>林珮馨</t>
+  </si>
+  <si>
+    <t>D092</t>
+  </si>
+  <si>
+    <t>陳秀珍</t>
+  </si>
+  <si>
+    <t>D096</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,6 +77,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="13.5"/>
+      <color theme="1"/>
+      <name val="Roboto"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -98,7 +92,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -106,15 +100,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFE0E0E0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,18 +438,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:AG14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:33">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -469,67 +476,67 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:33" ht="18">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
-        <v>0.3125</v>
-      </c>
-      <c r="C2" s="1">
+      <c r="B2" s="5">
+        <v>0.375</v>
+      </c>
+      <c r="C2" s="5">
         <v>0.41666666666666669</v>
       </c>
-      <c r="D2" s="1">
-        <v>0.42708333333333331</v>
-      </c>
-      <c r="E2" s="1">
+      <c r="D2" s="5">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="E2" s="5">
         <v>0.5</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="5">
         <v>0.54166666666666663</v>
       </c>
-      <c r="G2" s="1">
-        <v>0.64583333333333337</v>
-      </c>
-      <c r="H2" s="1">
+      <c r="G2" s="5">
         <v>0.65625</v>
       </c>
-      <c r="I2" s="1">
+      <c r="H2" s="5">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="I2" s="5">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:33" ht="18">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5">
+        <v>0.375</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0.4375</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="G3" s="5">
+        <v>0.65625</v>
+      </c>
+      <c r="H3" s="5">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="I3" s="5">
         <v>0.75</v>
       </c>
-      <c r="J2" s="1"/>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>0.35416666666666669</v>
-      </c>
-      <c r="C3" s="1">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0.42708333333333331</v>
-      </c>
-      <c r="E3" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="G3" s="1">
-        <v>0.64583333333333337</v>
-      </c>
-      <c r="H3" s="1">
-        <v>0.65625</v>
-      </c>
-      <c r="I3" s="1">
-        <v>0.77083333333333337</v>
-      </c>
       <c r="J3" s="1"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:33">
       <c r="C5" s="2">
         <v>44805</v>
       </c>
@@ -554,9 +561,76 @@
       <c r="J5" s="2">
         <v>44812</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" t="s">
+      <c r="K5" s="2">
+        <v>44813</v>
+      </c>
+      <c r="L5" s="2">
+        <v>44814</v>
+      </c>
+      <c r="M5" s="2">
+        <v>44815</v>
+      </c>
+      <c r="N5" s="2">
+        <v>44816</v>
+      </c>
+      <c r="O5" s="2">
+        <v>44817</v>
+      </c>
+      <c r="P5" s="2">
+        <v>44818</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>44819</v>
+      </c>
+      <c r="R5" s="2">
+        <v>44820</v>
+      </c>
+      <c r="S5" s="2">
+        <v>44821</v>
+      </c>
+      <c r="T5" s="2">
+        <v>44822</v>
+      </c>
+      <c r="U5" s="2">
+        <v>44823</v>
+      </c>
+      <c r="V5" s="2">
+        <v>44824</v>
+      </c>
+      <c r="W5" s="2">
+        <v>44825</v>
+      </c>
+      <c r="X5" s="2">
+        <v>44826</v>
+      </c>
+      <c r="Y5" s="2">
+        <v>44827</v>
+      </c>
+      <c r="Z5" s="2">
+        <v>44828</v>
+      </c>
+      <c r="AA5" s="2">
+        <v>44829</v>
+      </c>
+      <c r="AB5" s="2">
+        <v>44830</v>
+      </c>
+      <c r="AC5" s="2">
+        <v>44831</v>
+      </c>
+      <c r="AD5" s="2">
+        <v>44832</v>
+      </c>
+      <c r="AE5" s="2">
+        <v>44833</v>
+      </c>
+      <c r="AF5" s="2">
+        <v>44834</v>
+      </c>
+      <c r="AG5" s="2"/>
+    </row>
+    <row r="6" spans="1:33" ht="16.5">
+      <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B6" t="s">
@@ -584,7 +658,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:33">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -610,8 +684,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
-      <c r="A8" t="s">
+    <row r="8" spans="1:33" ht="16.5">
+      <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B8" t="s">
@@ -633,195 +707,40 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" t="s">
-        <v>1</v>
-      </c>
-      <c r="E10" t="s">
-        <v>2</v>
-      </c>
-      <c r="F10" t="s">
-        <v>1</v>
-      </c>
-      <c r="G10" t="s">
-        <v>2</v>
-      </c>
-      <c r="H10" t="s">
-        <v>1</v>
-      </c>
-      <c r="I10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11">
-        <v>1</v>
-      </c>
-      <c r="B11" s="1">
-        <v>0.3125</v>
-      </c>
-      <c r="C11" s="1">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="D11" s="1">
-        <v>0.42708333333333331</v>
-      </c>
-      <c r="E11" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="F11" s="1">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="G11" s="1">
-        <v>0.64583333333333337</v>
-      </c>
-      <c r="H11" s="1">
-        <v>0.65625</v>
-      </c>
-      <c r="I11" s="1">
-        <v>0.75</v>
-      </c>
+    <row r="10" spans="1:33">
+      <c r="A10" s="3"/>
+    </row>
+    <row r="11" spans="1:33">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:10">
-      <c r="A12">
-        <v>2</v>
-      </c>
-      <c r="B12" s="1">
-        <v>0.35416666666666669</v>
-      </c>
-      <c r="C12" s="1">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="D12" s="1">
-        <v>0.42708333333333331</v>
-      </c>
-      <c r="E12" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="F12" s="1">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="G12" s="1">
-        <v>0.64583333333333337</v>
-      </c>
-      <c r="H12" s="1">
-        <v>0.65625</v>
-      </c>
-      <c r="I12" s="1">
-        <v>0.77083333333333337</v>
-      </c>
+    <row r="12" spans="1:33">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="14" spans="1:10">
-      <c r="C14" s="2">
-        <v>44805</v>
-      </c>
-      <c r="D14" s="2">
-        <v>44806</v>
-      </c>
-      <c r="E14" s="2">
-        <v>44807</v>
-      </c>
-      <c r="F14" s="2">
-        <v>44808</v>
-      </c>
-      <c r="G14" s="2">
-        <v>44809</v>
-      </c>
-      <c r="H14" s="2">
-        <v>44810</v>
-      </c>
-      <c r="I14" s="2">
-        <v>44811</v>
-      </c>
-      <c r="J14" s="2">
-        <v>44812</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15">
-        <v>2</v>
-      </c>
-      <c r="G15">
-        <v>2</v>
-      </c>
-      <c r="H15">
-        <v>1</v>
-      </c>
-      <c r="I15">
-        <v>1</v>
-      </c>
-      <c r="J15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="F16">
-        <v>1</v>
-      </c>
-      <c r="G16">
-        <v>1</v>
-      </c>
-      <c r="I16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
-      <c r="A17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17">
-        <v>2</v>
-      </c>
-      <c r="F17">
-        <v>2</v>
-      </c>
-      <c r="G17">
-        <v>2</v>
-      </c>
-      <c r="I17">
-        <v>1</v>
-      </c>
-      <c r="J17">
-        <v>1</v>
-      </c>
+    <row r="14" spans="1:33">
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>